<commit_message>
maze6 expected step/path to be fixed
</commit_message>
<xml_diff>
--- a/dataAnalysis/MazeStepPath.xlsx
+++ b/dataAnalysis/MazeStepPath.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10092"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10092" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Maze4" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="172">
   <si>
     <t>T</t>
   </si>
@@ -346,14 +346,209 @@
     <t>(5-6)</t>
   </si>
   <si>
-    <t xml:space="preserve">		</t>
+    <t>(1-1)-&gt;(1-2)-&gt;(1-3)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(2-1)-&gt;(2-2)-&gt;(1-2)-&gt;(1-3)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(3-1)-&gt;(2-1)-&gt;(2-2)-&gt;(1-2)-&gt;(1-3)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(4-1)-&gt;(3-1)-&gt;(2-1)-&gt;(2-2)-&gt;(1-2)-&gt;(1-3)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(5-1)-&gt;(6-1)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(6-1)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(1-2)-&gt;(1-3)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(2-2)-&gt;(1-2)-&gt;(1-3)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(4-2)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(1-3)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(3-3)-&gt;(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(6-3)-&gt;(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(6-4)-&gt;(6-3)-&gt;(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(7-4)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(3-5)-&gt;(3-6)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(5-5)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(3-6)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(4-6)-&gt;(3-6)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(7-6)-&gt;(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(4-7)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(5-7)-&gt;(4-7)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(7-7)-&gt;(7-6)-&gt;(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(2-1)-&gt;(1-1)-&gt;(1-2)-&gt;(1-3)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(3-1)-&gt;(4-1)-&gt;(5-1)-&gt;(6-1)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(4-1)-&gt;(5-1)-&gt;(6-1)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(4-2)-&gt;(4-1)-&gt;(5-1)-&gt;(6-1)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(5-3)-&gt;(6-3)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(6-3)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(6-4)-&gt;(6-3)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(5-5)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(7-6)-&gt;(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(7-7)-&gt;(7-6)-&gt;(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(2-1)-&gt;(3-1)-&gt;(4-1)-&gt;(5-1)-&gt;(6-1)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(4-3)-&gt;(4-2)-&gt;(4-1)-&gt;(5-1)-&gt;(6-1)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(6-4)-&gt;(7-4)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(5-5)-&gt;(6-5)-&gt;(6-4)-&gt;(7-4)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(6-5)-&gt;(6-4)-&gt;(7-4)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(4-6)-&gt;(4-7)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(7-4)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(7-6)-&gt;(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(7-4)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(7-7)-&gt;(7-6)-&gt;(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(7-4)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(4-3)-&gt;(5-3)-&gt;(6-3)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(3-1)-&gt;(2-1)-&gt;(1-1)-&gt;(1-2)-&gt;(1-3)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(4-1)-&gt;(4-2)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(3-5)-&gt;(3-6)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(4-2)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(3-5)-&gt;(3-6)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(3-5)-&gt;(3-6)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(6-3)-&gt;(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(3-5)-&gt;(3-6)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(3-4)-&gt;(3-5)-&gt;(3-6)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(5-5)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(3-5)-&gt;(3-6)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(3-5)-&gt;(3-6)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(7-6)-&gt;(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(3-5)-&gt;(3-6)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,8 +556,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,6 +591,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -403,17 +610,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -728,7 +938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -1687,10 +1897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V55"/>
+  <dimension ref="A1:AA55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="X55" sqref="X55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1698,7 +1908,7 @@
     <col min="2" max="10" width="3.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C1">
         <v>1</v>
       </c>
@@ -1727,7 +1937,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1765,7 +1975,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1805,8 +2015,20 @@
       <c r="V3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="X3">
+        <v>6</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1841,13 +2063,25 @@
         <v>60</v>
       </c>
       <c r="U4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="V4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="X4">
+        <v>7</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1882,13 +2116,25 @@
         <v>60</v>
       </c>
       <c r="U5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="X5">
+        <v>5</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1928,8 +2174,20 @@
       <c r="V6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="X6">
+        <v>8</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1969,8 +2227,20 @@
       <c r="V7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="X7">
+        <v>4</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2005,13 +2275,25 @@
         <v>61</v>
       </c>
       <c r="U8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="V8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="X8">
+        <v>9</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2046,13 +2328,25 @@
         <v>61</v>
       </c>
       <c r="U9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="X9">
+        <v>3</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
@@ -2080,17 +2374,17 @@
       <c r="J10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="T10" t="s">
+      <c r="T10" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="U10" t="s">
-        <v>86</v>
-      </c>
-      <c r="V10">
+      <c r="U10" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="V10" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="T11" t="s">
         <v>63</v>
       </c>
@@ -2100,19 +2394,31 @@
       <c r="V11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="T12" t="s">
+      <c r="X11">
+        <v>2</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="T12" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="U12" t="s">
-        <v>86</v>
-      </c>
-      <c r="V12">
+      <c r="U12" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="V12" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="T13" t="s">
         <v>62</v>
       </c>
@@ -2122,8 +2428,20 @@
       <c r="V13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="X13">
+        <v>1</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="T14" t="s">
         <v>89</v>
       </c>
@@ -2133,8 +2451,20 @@
       <c r="V14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="X14">
+        <v>5</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="T15" t="s">
         <v>64</v>
       </c>
@@ -2144,52 +2474,100 @@
       <c r="V15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="X15">
+        <v>6</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="T16" t="s">
         <v>90</v>
       </c>
       <c r="U16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="V16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="20:22" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="X16">
+        <v>8</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T17" t="s">
         <v>90</v>
       </c>
       <c r="U17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T18" t="s">
+        <v>4</v>
+      </c>
+      <c r="X17">
+        <v>4</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T18" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="U18" t="s">
-        <v>87</v>
-      </c>
-      <c r="V18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="U18" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="V18" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T19" t="s">
         <v>91</v>
       </c>
       <c r="U19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V19">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="20:22" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="X19">
+        <v>1</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T20" t="s">
         <v>92</v>
       </c>
@@ -2199,8 +2577,20 @@
       <c r="V20">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X20">
+        <v>4</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T21" t="s">
         <v>93</v>
       </c>
@@ -2210,8 +2600,20 @@
       <c r="V21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X21">
+        <v>6</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T22" t="s">
         <v>69</v>
       </c>
@@ -2221,8 +2623,20 @@
       <c r="V22">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X22">
+        <v>7</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T23" t="s">
         <v>69</v>
       </c>
@@ -2232,8 +2646,20 @@
       <c r="V23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X23">
+        <v>5</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T24" t="s">
         <v>70</v>
       </c>
@@ -2243,8 +2669,20 @@
       <c r="V24">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X24">
+        <v>8</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T25" t="s">
         <v>70</v>
       </c>
@@ -2254,8 +2692,20 @@
       <c r="V25">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X25">
+        <v>4</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T26" t="s">
         <v>94</v>
       </c>
@@ -2265,8 +2715,20 @@
       <c r="V26">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X26">
+        <v>9</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T27" t="s">
         <v>94</v>
       </c>
@@ -2276,30 +2738,54 @@
       <c r="V27">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T28" t="s">
+      <c r="X27">
+        <v>3</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>146</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T28" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="U28" t="s">
-        <v>87</v>
-      </c>
-      <c r="V28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="U28" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="V28" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T29" t="s">
         <v>95</v>
       </c>
       <c r="U29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V29">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="20:22" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="X29">
+        <v>2</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T30" t="s">
         <v>71</v>
       </c>
@@ -2309,8 +2795,20 @@
       <c r="V30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X30">
+        <v>3</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T31" t="s">
         <v>72</v>
       </c>
@@ -2320,8 +2818,20 @@
       <c r="V31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X31">
+        <v>4</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T32" t="s">
         <v>73</v>
       </c>
@@ -2331,8 +2841,20 @@
       <c r="V32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X32">
+        <v>5</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T33" t="s">
         <v>76</v>
       </c>
@@ -2342,8 +2864,20 @@
       <c r="V33">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X33">
+        <v>10</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T34" t="s">
         <v>76</v>
       </c>
@@ -2353,30 +2887,54 @@
       <c r="V34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T35" t="s">
+      <c r="X34">
+        <v>4</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T35" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="U35" t="s">
-        <v>87</v>
-      </c>
-      <c r="V35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="U35" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="V35" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T36" t="s">
         <v>96</v>
       </c>
       <c r="U36" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V36">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="20:22" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="X36">
+        <v>3</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T37" t="s">
         <v>97</v>
       </c>
@@ -2386,8 +2944,20 @@
       <c r="V37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X37">
+        <v>2</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T38" t="s">
         <v>98</v>
       </c>
@@ -2397,8 +2967,20 @@
       <c r="V38">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X38">
+        <v>4</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T39" t="s">
         <v>79</v>
       </c>
@@ -2408,8 +2990,20 @@
       <c r="V39">
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X39">
+        <v>12</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T40" t="s">
         <v>79</v>
       </c>
@@ -2419,8 +3013,20 @@
       <c r="V40">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X40">
+        <v>6</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T41" t="s">
         <v>80</v>
       </c>
@@ -2430,8 +3036,20 @@
       <c r="V41">
         <v>11</v>
       </c>
-    </row>
-    <row r="42" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X41">
+        <v>11</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T42" t="s">
         <v>80</v>
       </c>
@@ -2441,8 +3059,20 @@
       <c r="V42">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X42">
+        <v>5</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T43" t="s">
         <v>59</v>
       </c>
@@ -2452,8 +3082,20 @@
       <c r="V43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X43">
+        <v>1</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T44" t="s">
         <v>82</v>
       </c>
@@ -2463,8 +3105,20 @@
       <c r="V44">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X44">
+        <v>3</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T45" t="s">
         <v>83</v>
       </c>
@@ -2474,8 +3128,20 @@
       <c r="V45">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X45">
+        <v>4</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T46" t="s">
         <v>84</v>
       </c>
@@ -2485,8 +3151,20 @@
       <c r="V46">
         <v>12</v>
       </c>
-    </row>
-    <row r="47" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X46">
+        <v>12</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T47" t="s">
         <v>84</v>
       </c>
@@ -2496,8 +3174,20 @@
       <c r="V47">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X47">
+        <v>6</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T48" t="s">
         <v>99</v>
       </c>
@@ -2507,8 +3197,20 @@
       <c r="V48">
         <v>13</v>
       </c>
-    </row>
-    <row r="49" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X48">
+        <v>13</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T49" t="s">
         <v>99</v>
       </c>
@@ -2518,8 +3220,20 @@
       <c r="V49">
         <v>7</v>
       </c>
-    </row>
-    <row r="50" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X49">
+        <v>7</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T50" t="s">
         <v>100</v>
       </c>
@@ -2529,8 +3243,20 @@
       <c r="V50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X50">
+        <v>1</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA50" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T51" t="s">
         <v>101</v>
       </c>
@@ -2540,8 +3266,20 @@
       <c r="V51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X51">
+        <v>2</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA51" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T52" t="s">
         <v>102</v>
       </c>
@@ -2551,8 +3289,20 @@
       <c r="V52">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X52">
+        <v>3</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA52" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T53" t="s">
         <v>103</v>
       </c>
@@ -2562,8 +3312,20 @@
       <c r="V53">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X53">
+        <v>4</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA53" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T54" t="s">
         <v>104</v>
       </c>
@@ -2573,8 +3335,20 @@
       <c r="V54">
         <v>14</v>
       </c>
-    </row>
-    <row r="55" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X54">
+        <v>14</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA54" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T55" t="s">
         <v>104</v>
       </c>
@@ -2583,6 +3357,18 @@
       </c>
       <c r="V55">
         <v>8</v>
+      </c>
+      <c r="X55">
+        <v>8</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA55" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2592,19 +3378,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V49"/>
+  <dimension ref="A1:AA65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="9" width="4.21875" customWidth="1"/>
     <col min="10" max="10" width="3.44140625" customWidth="1"/>
+    <col min="25" max="25" width="83" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C1">
         <v>1</v>
       </c>
@@ -2633,7 +3420,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2671,7 +3458,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2711,8 +3498,20 @@
       <c r="V3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="X3">
+        <v>6</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2752,8 +3551,20 @@
       <c r="V4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="X4">
+        <v>7</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2793,8 +3604,20 @@
       <c r="V5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="X5">
+        <v>8</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2834,8 +3657,20 @@
       <c r="V6">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="X6">
+        <v>9</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2875,8 +3710,20 @@
       <c r="V7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="X7">
+        <v>3</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2907,17 +3754,17 @@
       <c r="J8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T8" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="U8" t="s">
+      <c r="U8" s="5" t="s">
         <v>86</v>
       </c>
       <c r="V8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2954,11 +3801,23 @@
       <c r="U9" t="s">
         <v>87</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="X9">
+        <v>2</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
@@ -2986,371 +3845,641 @@
       <c r="J10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="T10" t="s">
+      <c r="X10">
+        <v>1</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X11">
+        <v>7</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X12">
+        <v>4</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X13">
+        <v>5</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="T14" t="s">
         <v>89</v>
       </c>
-      <c r="U10" t="s">
-        <v>86</v>
-      </c>
-      <c r="V10">
+      <c r="U14" t="s">
+        <v>86</v>
+      </c>
+      <c r="V14">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="T11" t="s">
+      <c r="X14">
+        <v>5</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="T15" t="s">
         <v>64</v>
       </c>
-      <c r="U11" t="s">
-        <v>86</v>
-      </c>
-      <c r="V11">
+      <c r="U15" t="s">
+        <v>86</v>
+      </c>
+      <c r="V15">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="T12" t="s">
+      <c r="X15">
+        <v>6</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="T16" t="s">
         <v>90</v>
       </c>
-      <c r="U12" t="s">
-        <v>86</v>
-      </c>
-      <c r="V12">
+      <c r="U16" t="s">
+        <v>86</v>
+      </c>
+      <c r="V16">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="T13" t="s">
+      <c r="X16">
+        <v>8</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z16" t="s">
         <v>90</v>
       </c>
-      <c r="U13" t="s">
-        <v>87</v>
-      </c>
-      <c r="V13">
+      <c r="AA16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T17" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="V17" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="T14" t="s">
+    <row r="18" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T18" t="s">
         <v>91</v>
       </c>
-      <c r="U14" t="s">
-        <v>87</v>
-      </c>
-      <c r="V14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="T15" t="s">
+      <c r="U18" t="s">
+        <v>87</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="X18">
+        <v>1</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z18" t="s">
         <v>91</v>
       </c>
-      <c r="U15" t="s">
-        <v>86</v>
-      </c>
-      <c r="V15">
+      <c r="AA18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T19" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="U19" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="V19" s="5">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="T16" t="s">
+      <c r="X19">
+        <v>4</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T20" t="s">
         <v>92</v>
       </c>
-      <c r="U16" t="s">
-        <v>86</v>
-      </c>
-      <c r="V16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T17" t="s">
+      <c r="U20" t="s">
+        <v>86</v>
+      </c>
+      <c r="V20">
+        <v>4</v>
+      </c>
+      <c r="X20">
+        <v>4</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T21" t="s">
         <v>93</v>
       </c>
-      <c r="U17" t="s">
-        <v>86</v>
-      </c>
-      <c r="V17">
+      <c r="U21" t="s">
+        <v>86</v>
+      </c>
+      <c r="V21">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T18" t="s">
+      <c r="X21">
+        <v>6</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T22" t="s">
         <v>69</v>
       </c>
-      <c r="U18" t="s">
-        <v>86</v>
-      </c>
-      <c r="V18">
+      <c r="U22" t="s">
+        <v>86</v>
+      </c>
+      <c r="V22">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T19" t="s">
+      <c r="X22">
+        <v>7</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z22" t="s">
         <v>69</v>
       </c>
-      <c r="U19" t="s">
-        <v>87</v>
-      </c>
-      <c r="V19">
+      <c r="AA22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T23" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="U23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="V23" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T20" t="s">
+    <row r="24" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T24" t="s">
         <v>70</v>
       </c>
-      <c r="U20" t="s">
-        <v>86</v>
-      </c>
-      <c r="V20">
+      <c r="U24" t="s">
+        <v>86</v>
+      </c>
+      <c r="V24">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T21" t="s">
+      <c r="X24">
+        <v>8</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z24" t="s">
         <v>70</v>
       </c>
-      <c r="U21" t="s">
-        <v>87</v>
-      </c>
-      <c r="V21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T22" t="s">
+      <c r="AA24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T25" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="U25" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="V25" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T26" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="U22" t="s">
-        <v>87</v>
-      </c>
-      <c r="V22">
+      <c r="U26" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="V26" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T23" t="s">
+    <row r="27" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T27" t="s">
         <v>94</v>
       </c>
-      <c r="U23" t="s">
-        <v>86</v>
-      </c>
-      <c r="V23">
+      <c r="U27" t="s">
+        <v>86</v>
+      </c>
+      <c r="V27">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T24" t="s">
+      <c r="X27">
+        <v>9</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T28" t="s">
         <v>95</v>
       </c>
-      <c r="U24" t="s">
-        <v>87</v>
-      </c>
-      <c r="V24">
+      <c r="U28" t="s">
+        <v>87</v>
+      </c>
+      <c r="V28">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T25" t="s">
+      <c r="X28">
+        <v>2</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z28" t="s">
         <v>95</v>
       </c>
-      <c r="U25" t="s">
-        <v>86</v>
-      </c>
-      <c r="V25">
+      <c r="AA28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T29" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="U29" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="V29" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T26" t="s">
+      <c r="X29">
+        <v>4</v>
+      </c>
+      <c r="Y29" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="X30">
+        <v>3</v>
+      </c>
+      <c r="Y30" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="X31">
+        <v>5</v>
+      </c>
+      <c r="Y31" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T32" t="s">
         <v>71</v>
       </c>
-      <c r="U26" t="s">
-        <v>86</v>
-      </c>
-      <c r="V26">
+      <c r="U32" t="s">
+        <v>86</v>
+      </c>
+      <c r="V32">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T27" t="s">
+      <c r="X32">
+        <v>3</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T33" t="s">
         <v>72</v>
       </c>
-      <c r="U27" t="s">
-        <v>86</v>
-      </c>
-      <c r="V27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T28" t="s">
+      <c r="U33" t="s">
+        <v>86</v>
+      </c>
+      <c r="V33">
+        <v>4</v>
+      </c>
+      <c r="X33">
+        <v>4</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T34" t="s">
         <v>73</v>
       </c>
-      <c r="U28" t="s">
-        <v>86</v>
-      </c>
-      <c r="V28">
+      <c r="U34" t="s">
+        <v>86</v>
+      </c>
+      <c r="V34">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T29" t="s">
+      <c r="X34">
+        <v>5</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T35" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="U29" t="s">
-        <v>87</v>
-      </c>
-      <c r="V29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T30" t="s">
+      <c r="U35" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="V35" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T36" t="s">
         <v>76</v>
       </c>
-      <c r="U30" t="s">
-        <v>86</v>
-      </c>
-      <c r="V30">
+      <c r="U36" t="s">
+        <v>86</v>
+      </c>
+      <c r="V36" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T31" t="s">
+      <c r="X36">
+        <v>10</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T37" t="s">
         <v>96</v>
       </c>
-      <c r="U31" t="s">
-        <v>87</v>
-      </c>
-      <c r="V31">
+      <c r="U37" t="s">
+        <v>87</v>
+      </c>
+      <c r="V37">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T32" t="s">
+      <c r="X37">
+        <v>3</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z37" t="s">
         <v>96</v>
       </c>
-      <c r="U32" t="s">
-        <v>86</v>
-      </c>
-      <c r="V32">
+      <c r="AA37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T38" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="U38" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="V38" s="5">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T33" t="s">
+    <row r="39" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T39" t="s">
         <v>97</v>
       </c>
-      <c r="U33" t="s">
-        <v>86</v>
-      </c>
-      <c r="V33">
+      <c r="U39" t="s">
+        <v>86</v>
+      </c>
+      <c r="V39">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T34" t="s">
+      <c r="X39">
+        <v>4</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T40" t="s">
         <v>98</v>
       </c>
-      <c r="U34" t="s">
-        <v>86</v>
-      </c>
-      <c r="V34">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T35" t="s">
+      <c r="U40" t="s">
+        <v>86</v>
+      </c>
+      <c r="V40">
+        <v>4</v>
+      </c>
+      <c r="X40">
+        <v>4</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T41" t="s">
         <v>79</v>
       </c>
-      <c r="U35" t="s">
-        <v>86</v>
-      </c>
-      <c r="V35">
+      <c r="U41" t="s">
+        <v>86</v>
+      </c>
+      <c r="V41">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T36" t="s">
+      <c r="X41">
+        <v>2</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T42" t="s">
         <v>80</v>
       </c>
-      <c r="U36" t="s">
-        <v>87</v>
-      </c>
-      <c r="V36">
+      <c r="U42" t="s">
+        <v>87</v>
+      </c>
+      <c r="V42">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T37" t="s">
+      <c r="X42">
+        <v>4</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T43" t="s">
         <v>80</v>
-      </c>
-      <c r="U37" t="s">
-        <v>86</v>
-      </c>
-      <c r="V37">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T38" t="s">
-        <v>59</v>
-      </c>
-      <c r="U38" t="s">
-        <v>86</v>
-      </c>
-      <c r="V38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T39" t="s">
-        <v>82</v>
-      </c>
-      <c r="U39" t="s">
-        <v>86</v>
-      </c>
-      <c r="V39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T40" t="s">
-        <v>83</v>
-      </c>
-      <c r="U40" t="s">
-        <v>86</v>
-      </c>
-      <c r="V40">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T41" t="s">
-        <v>105</v>
-      </c>
-      <c r="U41" t="s">
-        <v>86</v>
-      </c>
-      <c r="V41">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T42" t="s">
-        <v>84</v>
-      </c>
-      <c r="U42" t="s">
-        <v>86</v>
-      </c>
-      <c r="V42">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T43" t="s">
-        <v>99</v>
       </c>
       <c r="U43" t="s">
         <v>86</v>
@@ -3358,65 +4487,424 @@
       <c r="V43">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="20:22" x14ac:dyDescent="0.3">
+      <c r="X43">
+        <v>12</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="20:27" x14ac:dyDescent="0.3">
       <c r="T44" t="s">
+        <v>59</v>
+      </c>
+      <c r="U44" t="s">
+        <v>86</v>
+      </c>
+      <c r="V44">
+        <v>1</v>
+      </c>
+      <c r="X44">
+        <v>11</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T45" t="s">
+        <v>82</v>
+      </c>
+      <c r="U45" t="s">
+        <v>86</v>
+      </c>
+      <c r="V45">
+        <v>3</v>
+      </c>
+      <c r="X45">
+        <v>6</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T46" t="s">
+        <v>83</v>
+      </c>
+      <c r="U46" t="s">
+        <v>86</v>
+      </c>
+      <c r="V46">
+        <v>4</v>
+      </c>
+      <c r="X46">
+        <v>5</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T47" t="s">
+        <v>105</v>
+      </c>
+      <c r="U47" t="s">
+        <v>86</v>
+      </c>
+      <c r="V47">
+        <v>5</v>
+      </c>
+      <c r="X47">
+        <v>6</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T48" t="s">
+        <v>84</v>
+      </c>
+      <c r="U48" t="s">
+        <v>86</v>
+      </c>
+      <c r="V48">
+        <v>6</v>
+      </c>
+      <c r="X48">
+        <v>5</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T49" t="s">
+        <v>99</v>
+      </c>
+      <c r="U49" t="s">
+        <v>86</v>
+      </c>
+      <c r="V49">
+        <v>7</v>
+      </c>
+      <c r="X49">
+        <v>1</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T50" t="s">
         <v>100</v>
       </c>
-      <c r="U44" t="s">
-        <v>86</v>
-      </c>
-      <c r="V44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T45" t="s">
+      <c r="U50" t="s">
+        <v>86</v>
+      </c>
+      <c r="V50">
+        <v>1</v>
+      </c>
+      <c r="X50">
+        <v>3</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA50" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T51" t="s">
         <v>101</v>
       </c>
-      <c r="U45" t="s">
-        <v>86</v>
-      </c>
-      <c r="V45">
+      <c r="U51" t="s">
+        <v>86</v>
+      </c>
+      <c r="V51">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T46" t="s">
+      <c r="X51">
+        <v>4</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA51" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T52" t="s">
         <v>102</v>
       </c>
-      <c r="U46" t="s">
-        <v>86</v>
-      </c>
-      <c r="V46">
+      <c r="U52" t="s">
+        <v>86</v>
+      </c>
+      <c r="V52">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T47" t="s">
+      <c r="X52">
+        <v>12</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA52" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T53" t="s">
         <v>103</v>
       </c>
-      <c r="U47" t="s">
-        <v>86</v>
-      </c>
-      <c r="V47">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="20:22" x14ac:dyDescent="0.3">
-      <c r="T48" t="s">
+      <c r="U53" t="s">
+        <v>86</v>
+      </c>
+      <c r="V53">
+        <v>4</v>
+      </c>
+      <c r="X53">
+        <v>13</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA53" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="T54" t="s">
         <v>104</v>
       </c>
-      <c r="U48" t="s">
-        <v>86</v>
-      </c>
-      <c r="V48">
+      <c r="U54" t="s">
+        <v>86</v>
+      </c>
+      <c r="V54">
         <v>8</v>
       </c>
-    </row>
-    <row r="49" spans="20:20" x14ac:dyDescent="0.3">
-      <c r="T49" t="s">
-        <v>106</v>
+      <c r="X54">
+        <v>6</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA54" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="X55">
+        <v>7</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA55" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="X56">
+        <v>4</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z56" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA56" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="X57">
+        <v>6</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z57" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="X58">
+        <v>7</v>
+      </c>
+      <c r="Y58" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA58" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="X59">
+        <v>1</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z59" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA59" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="X60">
+        <v>2</v>
+      </c>
+      <c r="Y60" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z60" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA60" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="61" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="X61">
+        <v>3</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z61" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA61" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="X62">
+        <v>4</v>
+      </c>
+      <c r="Y62" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z62" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA62" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="X63">
+        <v>14</v>
+      </c>
+      <c r="Y63" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z63" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA63" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="20:27" x14ac:dyDescent="0.3">
+      <c r="X64">
+        <v>8</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z64" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA64" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="24:27" x14ac:dyDescent="0.3">
+      <c r="X65">
+        <v>8</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z65" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA65" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refined stats, get first 30 location in path if openstate cannot reach final state within 100 steps
</commit_message>
<xml_diff>
--- a/dataAnalysis/MazeStepPath.xlsx
+++ b/dataAnalysis/MazeStepPath.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10092" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10092" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Maze4" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="175">
   <si>
     <t>T</t>
   </si>
@@ -355,9 +355,6 @@
     <t>(3-1)-&gt;(2-1)-&gt;(2-2)-&gt;(1-2)-&gt;(1-3)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
   </si>
   <si>
-    <t>(4-1)-&gt;(3-1)-&gt;(2-1)-&gt;(2-2)-&gt;(1-2)-&gt;(1-3)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
-  </si>
-  <si>
     <t>(5-1)-&gt;(6-1)-&gt;(7-1)</t>
   </si>
   <si>
@@ -388,9 +385,6 @@
     <t>(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
   </si>
   <si>
-    <t>(6-3)-&gt;(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
-  </si>
-  <si>
     <t>(7-3)-&gt;(7-2)-&gt;(7-1)</t>
   </si>
   <si>
@@ -415,9 +409,6 @@
     <t>(3-5)-&gt;(3-6)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
   </si>
   <si>
-    <t>(5-5)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
-  </si>
-  <si>
     <t>(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
   </si>
   <si>
@@ -430,12 +421,6 @@
     <t>(4-6)-&gt;(3-6)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
   </si>
   <si>
-    <t>(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
-  </si>
-  <si>
-    <t>(7-6)-&gt;(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(2-4)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
-  </si>
-  <si>
     <t>(2-7)-&gt;(1-7)</t>
   </si>
   <si>
@@ -472,48 +457,27 @@
     <t>(6-4)-&gt;(6-3)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
   </si>
   <si>
-    <t>(5-5)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
-  </si>
-  <si>
     <t>(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
   </si>
   <si>
     <t>(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
   </si>
   <si>
-    <t>(7-6)-&gt;(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
-  </si>
-  <si>
     <t>(7-7)-&gt;(7-6)-&gt;(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
   </si>
   <si>
     <t>(2-1)-&gt;(3-1)-&gt;(4-1)-&gt;(5-1)-&gt;(6-1)-&gt;(7-1)</t>
   </si>
   <si>
-    <t>(4-3)-&gt;(4-2)-&gt;(4-1)-&gt;(5-1)-&gt;(6-1)-&gt;(7-1)</t>
-  </si>
-  <si>
-    <t>(6-4)-&gt;(7-4)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
-  </si>
-  <si>
     <t>(5-5)-&gt;(6-5)-&gt;(6-4)-&gt;(7-4)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
   </si>
   <si>
-    <t>(6-5)-&gt;(6-4)-&gt;(7-4)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
-  </si>
-  <si>
     <t>(4-6)-&gt;(4-7)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
   </si>
   <si>
-    <t>(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(7-4)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
-  </si>
-  <si>
     <t>(7-6)-&gt;(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(7-4)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
   </si>
   <si>
-    <t>(7-7)-&gt;(7-6)-&gt;(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(7-4)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
-  </si>
-  <si>
     <t>(4-3)-&gt;(5-3)-&gt;(6-3)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
   </si>
   <si>
@@ -542,13 +506,58 @@
   </si>
   <si>
     <t>(7-6)-&gt;(6-6)-&gt;(6-5)-&gt;(6-4)-&gt;(6-3)-&gt;(5-3)-&gt;(4-3)-&gt;(3-3)-&gt;(3-4)-&gt;(3-5)-&gt;(3-6)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>steps</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>(4-1)-&gt;(3-1)-&gt;(2-1)-&gt;(1-1)-&gt;(1-2)-&gt;(1-3)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(5-1)-&gt;(4-1)-&gt;(3-1)-&gt;(2-1)-&gt;(2-2)-&gt;(1-2)-&gt;(1-3)-&gt;(1-4)-&gt;(1-5)-&gt;(1-6)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(4-2)-&gt;(4-3)-&gt;(5-3)-&gt;(6-3)-&gt;(7-3)-&gt;(7-2)-&gt;(7-1)</t>
+  </si>
+  <si>
+    <t>(6-3)-&gt;(6-4)-&gt;(6-5)-&gt;(6-6)-&gt;(5-6)-&gt;(5-7)-&gt;(4-7)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(6-4)-&gt;(6-5)-&gt;(6-6)-&gt;(5-6)-&gt;(5-7)-&gt;(4-7)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(7-4)-&gt;(6-4)-&gt;(6-5)-&gt;(6-6)-&gt;(5-6)-&gt;(5-7)-&gt;(4-7)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(5-5)-&gt;(5-6)-&gt;(5-7)-&gt;(4-7)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(6-5)-&gt;(6-6)-&gt;(5-6)-&gt;(5-7)-&gt;(4-7)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(5-6)-&gt;(5-7)-&gt;(4-7)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(6-6)-&gt;(5-6)-&gt;(5-7)-&gt;(4-7)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(7-6)-&gt;(6-6)-&gt;(5-6)-&gt;(5-7)-&gt;(4-7)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
+  </si>
+  <si>
+    <t>(7-7)-&gt;(7-6)-&gt;(6-6)-&gt;(5-6)-&gt;(5-7)-&gt;(4-7)-&gt;(3-7)-&gt;(2-7)-&gt;(1-7)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -563,8 +572,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -600,12 +631,92 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -614,13 +725,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1899,7 +2027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="X55" sqref="X55"/>
     </sheetView>
   </sheetViews>
@@ -2125,7 +2253,7 @@
         <v>5</v>
       </c>
       <c r="Y5" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="Z5" t="s">
         <v>60</v>
@@ -2178,7 +2306,7 @@
         <v>8</v>
       </c>
       <c r="Y6" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="Z6" t="s">
         <v>88</v>
@@ -2231,7 +2359,7 @@
         <v>4</v>
       </c>
       <c r="Y7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="Z7" t="s">
         <v>88</v>
@@ -2284,7 +2412,7 @@
         <v>9</v>
       </c>
       <c r="Y8" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="Z8" t="s">
         <v>61</v>
@@ -2337,7 +2465,7 @@
         <v>3</v>
       </c>
       <c r="Y9" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="Z9" t="s">
         <v>61</v>
@@ -2398,7 +2526,7 @@
         <v>2</v>
       </c>
       <c r="Y11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Z11" t="s">
         <v>63</v>
@@ -2432,7 +2560,7 @@
         <v>1</v>
       </c>
       <c r="Y13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Z13" t="s">
         <v>62</v>
@@ -2455,7 +2583,7 @@
         <v>5</v>
       </c>
       <c r="Y14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Z14" t="s">
         <v>89</v>
@@ -2478,7 +2606,7 @@
         <v>6</v>
       </c>
       <c r="Y15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Z15" t="s">
         <v>64</v>
@@ -2501,7 +2629,7 @@
         <v>8</v>
       </c>
       <c r="Y16" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="Z16" t="s">
         <v>90</v>
@@ -2524,7 +2652,7 @@
         <v>4</v>
       </c>
       <c r="Y17" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="Z17" t="s">
         <v>90</v>
@@ -2558,7 +2686,7 @@
         <v>1</v>
       </c>
       <c r="Y19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Z19" t="s">
         <v>91</v>
@@ -2581,7 +2709,7 @@
         <v>4</v>
       </c>
       <c r="Y20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Z20" t="s">
         <v>92</v>
@@ -2604,7 +2732,7 @@
         <v>6</v>
       </c>
       <c r="Y21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Z21" t="s">
         <v>93</v>
@@ -2627,7 +2755,7 @@
         <v>7</v>
       </c>
       <c r="Y22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z22" t="s">
         <v>69</v>
@@ -2650,7 +2778,7 @@
         <v>5</v>
       </c>
       <c r="Y23" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="Z23" t="s">
         <v>69</v>
@@ -2673,7 +2801,7 @@
         <v>8</v>
       </c>
       <c r="Y24" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="Z24" t="s">
         <v>70</v>
@@ -2696,7 +2824,7 @@
         <v>4</v>
       </c>
       <c r="Y25" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="Z25" t="s">
         <v>70</v>
@@ -2719,7 +2847,7 @@
         <v>9</v>
       </c>
       <c r="Y26" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="Z26" t="s">
         <v>94</v>
@@ -2742,7 +2870,7 @@
         <v>3</v>
       </c>
       <c r="Y27" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="Z27" t="s">
         <v>94</v>
@@ -2776,7 +2904,7 @@
         <v>2</v>
       </c>
       <c r="Y29" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Z29" t="s">
         <v>95</v>
@@ -2799,7 +2927,7 @@
         <v>3</v>
       </c>
       <c r="Y30" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Z30" t="s">
         <v>71</v>
@@ -2822,7 +2950,7 @@
         <v>4</v>
       </c>
       <c r="Y31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="Z31" t="s">
         <v>72</v>
@@ -2845,7 +2973,7 @@
         <v>5</v>
       </c>
       <c r="Y32" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="Z32" t="s">
         <v>73</v>
@@ -2868,7 +2996,7 @@
         <v>10</v>
       </c>
       <c r="Y33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Z33" t="s">
         <v>76</v>
@@ -2891,7 +3019,7 @@
         <v>4</v>
       </c>
       <c r="Y34" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="Z34" t="s">
         <v>76</v>
@@ -2925,7 +3053,7 @@
         <v>3</v>
       </c>
       <c r="Y36" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="Z36" t="s">
         <v>96</v>
@@ -2948,7 +3076,7 @@
         <v>2</v>
       </c>
       <c r="Y37" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Z37" t="s">
         <v>97</v>
@@ -2971,7 +3099,7 @@
         <v>4</v>
       </c>
       <c r="Y38" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Z38" t="s">
         <v>98</v>
@@ -2994,7 +3122,7 @@
         <v>12</v>
       </c>
       <c r="Y39" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="Z39" t="s">
         <v>79</v>
@@ -3017,7 +3145,7 @@
         <v>6</v>
       </c>
       <c r="Y40" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="Z40" t="s">
         <v>79</v>
@@ -3040,7 +3168,7 @@
         <v>11</v>
       </c>
       <c r="Y41" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Z41" t="s">
         <v>80</v>
@@ -3063,7 +3191,7 @@
         <v>5</v>
       </c>
       <c r="Y42" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="Z42" t="s">
         <v>80</v>
@@ -3086,7 +3214,7 @@
         <v>1</v>
       </c>
       <c r="Y43" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Z43" t="s">
         <v>59</v>
@@ -3109,7 +3237,7 @@
         <v>3</v>
       </c>
       <c r="Y44" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Z44" t="s">
         <v>82</v>
@@ -3132,7 +3260,7 @@
         <v>4</v>
       </c>
       <c r="Y45" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="Z45" t="s">
         <v>83</v>
@@ -3155,7 +3283,7 @@
         <v>12</v>
       </c>
       <c r="Y46" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="Z46" t="s">
         <v>84</v>
@@ -3178,7 +3306,7 @@
         <v>6</v>
       </c>
       <c r="Y47" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="Z47" t="s">
         <v>84</v>
@@ -3201,7 +3329,7 @@
         <v>13</v>
       </c>
       <c r="Y48" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="Z48" t="s">
         <v>99</v>
@@ -3224,7 +3352,7 @@
         <v>7</v>
       </c>
       <c r="Y49" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="Z49" t="s">
         <v>99</v>
@@ -3247,7 +3375,7 @@
         <v>1</v>
       </c>
       <c r="Y50" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="Z50" t="s">
         <v>100</v>
@@ -3270,7 +3398,7 @@
         <v>2</v>
       </c>
       <c r="Y51" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="Z51" t="s">
         <v>101</v>
@@ -3293,7 +3421,7 @@
         <v>3</v>
       </c>
       <c r="Y52" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="Z52" t="s">
         <v>102</v>
@@ -3316,7 +3444,7 @@
         <v>4</v>
       </c>
       <c r="Y53" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="Z53" t="s">
         <v>103</v>
@@ -3339,7 +3467,7 @@
         <v>14</v>
       </c>
       <c r="Y54" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="Z54" t="s">
         <v>104</v>
@@ -3362,7 +3490,7 @@
         <v>8</v>
       </c>
       <c r="Y55" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="Z55" t="s">
         <v>104</v>
@@ -3378,20 +3506,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA65"/>
+  <dimension ref="A1:AB48"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="9" width="4.21875" customWidth="1"/>
     <col min="10" max="10" width="3.44140625" customWidth="1"/>
-    <col min="25" max="25" width="83" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C1">
         <v>1</v>
       </c>
@@ -3420,7 +3548,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -3457,8 +3585,23 @@
       <c r="V2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X2" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y2" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA2" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB2" s="14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3498,20 +3641,26 @@
       <c r="V3">
         <v>6</v>
       </c>
-      <c r="X3">
+      <c r="X3" s="15">
         <v>6</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Y3" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="Z3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="Z3" s="17" t="str">
+        <f>LEFT(Y3,5)</f>
+        <v>(1-1)</v>
+      </c>
+      <c r="AA3" s="17" t="str">
+        <f>RIGHT(Y3,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB3" s="18" t="str">
+        <f>RIGHT(Z3,2)</f>
+        <v>1)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3551,20 +3700,26 @@
       <c r="V4">
         <v>7</v>
       </c>
-      <c r="X4">
+      <c r="X4" s="19">
         <v>7</v>
       </c>
-      <c r="Y4" t="s">
-        <v>107</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="Y4" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z4" s="21" t="str">
+        <f>LEFT(Y4,5)</f>
+        <v>(2-1)</v>
+      </c>
+      <c r="AA4" s="21" t="str">
+        <f>RIGHT(Y4,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB4" s="22" t="str">
+        <f>RIGHT(Z4,2)</f>
+        <v>1)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3604,20 +3759,26 @@
       <c r="V5">
         <v>8</v>
       </c>
-      <c r="X5">
+      <c r="X5" s="15">
         <v>8</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Y5" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="Z5" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="Z5" s="17" t="str">
+        <f>LEFT(Y5,5)</f>
+        <v>(3-1)</v>
+      </c>
+      <c r="AA5" s="17" t="str">
+        <f>RIGHT(Y5,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB5" s="18" t="str">
+        <f>RIGHT(Z5,2)</f>
+        <v>1)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3657,20 +3818,26 @@
       <c r="V6">
         <v>9</v>
       </c>
-      <c r="X6">
+      <c r="X6" s="19">
         <v>9</v>
       </c>
-      <c r="Y6" t="s">
-        <v>109</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="Y6" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z6" s="21" t="str">
+        <f>LEFT(Y6,5)</f>
+        <v>(4-1)</v>
+      </c>
+      <c r="AA6" s="21" t="str">
+        <f>RIGHT(Y6,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB6" s="22" t="str">
+        <f>RIGHT(Z6,2)</f>
+        <v>1)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3710,20 +3877,13 @@
       <c r="V7">
         <v>7</v>
       </c>
-      <c r="X7">
-        <v>3</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>143</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X7" s="15"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="17"/>
+      <c r="AA7" s="17"/>
+      <c r="AB7" s="18"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3754,17 +3914,35 @@
       <c r="J8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="T8" s="5" t="s">
+      <c r="T8" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="U8" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="V8">
+      <c r="U8" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="V8" s="11">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X8" s="19">
+        <v>10</v>
+      </c>
+      <c r="Y8" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z8" s="21" t="str">
+        <f>LEFT(Y8,5)</f>
+        <v>(5-1)</v>
+      </c>
+      <c r="AA8" s="21" t="str">
+        <f>RIGHT(Y8,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB8" s="22" t="str">
+        <f>RIGHT(Z8,2)</f>
+        <v>1)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3795,1116 +3973,1136 @@
       <c r="J9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="U9" t="s">
+      <c r="U9" s="5" t="s">
         <v>87</v>
       </c>
       <c r="V9" s="5">
         <v>8</v>
       </c>
-      <c r="X9">
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="T10" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="U10" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V10" s="11">
+        <v>5</v>
+      </c>
+      <c r="X10" s="15">
+        <v>5</v>
+      </c>
+      <c r="Y10" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z10" s="17" t="str">
+        <f>LEFT(Y10,5)</f>
+        <v>(1-2)</v>
+      </c>
+      <c r="AA10" s="17" t="str">
+        <f>RIGHT(Y10,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB10" s="18" t="str">
+        <f>RIGHT(Z10,2)</f>
+        <v>2)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="T11" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="U11" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V11" s="11">
+        <v>6</v>
+      </c>
+      <c r="X11" s="19">
+        <v>6</v>
+      </c>
+      <c r="Y11" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z11" s="21" t="str">
+        <f>LEFT(Y11,5)</f>
+        <v>(2-2)</v>
+      </c>
+      <c r="AA11" s="21" t="str">
+        <f>RIGHT(Y11,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB11" s="22" t="str">
+        <f>RIGHT(Z11,2)</f>
+        <v>2)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="T12" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="U12" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V12" s="11">
+        <v>8</v>
+      </c>
+      <c r="X12" s="15">
+        <v>8</v>
+      </c>
+      <c r="Y12" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z12" s="17" t="str">
+        <f>LEFT(Y12,5)</f>
+        <v>(4-2)</v>
+      </c>
+      <c r="AA12" s="17" t="str">
+        <f>RIGHT(Y12,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB12" s="18" t="str">
+        <f>RIGHT(Z12,2)</f>
+        <v>2)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="T13" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="U13" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="V13" s="10">
+        <v>6</v>
+      </c>
+      <c r="X13" s="19">
+        <v>6</v>
+      </c>
+      <c r="Y13" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z13" s="21" t="str">
+        <f>LEFT(Y13,5)</f>
+        <v>(4-2)</v>
+      </c>
+      <c r="AA13" s="21" t="str">
+        <f>RIGHT(Y13,5)</f>
+        <v>(7-1)</v>
+      </c>
+      <c r="AB13" s="22" t="str">
+        <f>RIGHT(Z13,2)</f>
+        <v>2)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="T14" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="U14" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="V14" s="11">
+        <v>1</v>
+      </c>
+      <c r="X14" s="15">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z14" s="17" t="str">
+        <f>LEFT(Y14,5)</f>
+        <v>(7-2)</v>
+      </c>
+      <c r="AA14" s="17" t="str">
+        <f>RIGHT(Y14,5)</f>
+        <v>(7-1)</v>
+      </c>
+      <c r="AB14" s="18" t="str">
+        <f>RIGHT(Z14,2)</f>
+        <v>2)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="T15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="U15" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="V15" s="10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="T16" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="U16" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V16" s="11">
+        <v>4</v>
+      </c>
+      <c r="X16" s="19">
+        <v>4</v>
+      </c>
+      <c r="Y16" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z16" s="21" t="str">
+        <f>LEFT(Y16,5)</f>
+        <v>(1-3)</v>
+      </c>
+      <c r="AA16" s="21" t="str">
+        <f>RIGHT(Y16,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB16" s="22" t="str">
+        <f>RIGHT(Z16,2)</f>
+        <v>3)</v>
+      </c>
+    </row>
+    <row r="17" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T17" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="U17" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V17" s="11">
+        <v>6</v>
+      </c>
+      <c r="X17" s="15">
+        <v>6</v>
+      </c>
+      <c r="Y17" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z17" s="17" t="str">
+        <f>LEFT(Y17,5)</f>
+        <v>(3-3)</v>
+      </c>
+      <c r="AA17" s="17" t="str">
+        <f>RIGHT(Y17,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB17" s="18" t="str">
+        <f>RIGHT(Z17,2)</f>
+        <v>3)</v>
+      </c>
+    </row>
+    <row r="18" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T18" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="U18" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V18" s="11">
+        <v>7</v>
+      </c>
+      <c r="X18" s="15">
+        <v>7</v>
+      </c>
+      <c r="Y18" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z18" s="17" t="str">
+        <f>LEFT(Y18,5)</f>
+        <v>(4-3)</v>
+      </c>
+      <c r="AA18" s="17" t="str">
+        <f>RIGHT(Y18,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB18" s="18" t="str">
+        <f>RIGHT(Z18,2)</f>
+        <v>3)</v>
+      </c>
+    </row>
+    <row r="19" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T19" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="U19" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="V19" s="10">
+        <v>5</v>
+      </c>
+      <c r="X19" s="19">
+        <v>5</v>
+      </c>
+      <c r="Y19" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z19" s="21" t="str">
+        <f>LEFT(Y19,5)</f>
+        <v>(4-3)</v>
+      </c>
+      <c r="AA19" s="21" t="str">
+        <f>RIGHT(Y19,5)</f>
+        <v>(7-1)</v>
+      </c>
+      <c r="AB19" s="22" t="str">
+        <f>RIGHT(Z19,2)</f>
+        <v>3)</v>
+      </c>
+    </row>
+    <row r="20" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T20" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="U20" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V20" s="11">
+        <v>8</v>
+      </c>
+      <c r="X20" s="15">
+        <v>8</v>
+      </c>
+      <c r="Y20" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z20" s="17" t="str">
+        <f>LEFT(Y20,5)</f>
+        <v>(5-3)</v>
+      </c>
+      <c r="AA20" s="17" t="str">
+        <f>RIGHT(Y20,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB20" s="18" t="str">
+        <f>RIGHT(Z20,2)</f>
+        <v>3)</v>
+      </c>
+    </row>
+    <row r="21" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T21" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="U21" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="V21" s="10">
+        <v>4</v>
+      </c>
+      <c r="X21" s="19">
+        <v>4</v>
+      </c>
+      <c r="Y21" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z21" s="21" t="str">
+        <f>LEFT(Y21,5)</f>
+        <v>(5-3)</v>
+      </c>
+      <c r="AA21" s="21" t="str">
+        <f>RIGHT(Y21,5)</f>
+        <v>(7-1)</v>
+      </c>
+      <c r="AB21" s="22" t="str">
+        <f>RIGHT(Z21,2)</f>
+        <v>3)</v>
+      </c>
+    </row>
+    <row r="22" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T22" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="U22" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V22" s="11">
+        <v>9</v>
+      </c>
+      <c r="X22" s="15">
+        <v>9</v>
+      </c>
+      <c r="Y22" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z22" s="17" t="str">
+        <f>LEFT(Y22,5)</f>
+        <v>(6-3)</v>
+      </c>
+      <c r="AA22" s="17" t="str">
+        <f>RIGHT(Y22,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB22" s="18" t="str">
+        <f>RIGHT(Z22,2)</f>
+        <v>3)</v>
+      </c>
+    </row>
+    <row r="23" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T23" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="U23" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="V23" s="10">
+        <v>3</v>
+      </c>
+      <c r="X23" s="19">
+        <v>3</v>
+      </c>
+      <c r="Y23" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z23" s="21" t="str">
+        <f>LEFT(Y23,5)</f>
+        <v>(6-3)</v>
+      </c>
+      <c r="AA23" s="21" t="str">
+        <f>RIGHT(Y23,5)</f>
+        <v>(7-1)</v>
+      </c>
+      <c r="AB23" s="22" t="str">
+        <f>RIGHT(Z23,2)</f>
+        <v>3)</v>
+      </c>
+    </row>
+    <row r="24" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T24" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="U24" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="V24" s="11">
         <v>2</v>
       </c>
-      <c r="Y9" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA9" t="s">
+      <c r="X24" s="15">
+        <v>2</v>
+      </c>
+      <c r="Y24" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z24" s="17" t="str">
+        <f>LEFT(Y24,5)</f>
+        <v>(7-3)</v>
+      </c>
+      <c r="AA24" s="17" t="str">
+        <f>RIGHT(Y24,5)</f>
+        <v>(7-1)</v>
+      </c>
+      <c r="AB24" s="18" t="str">
+        <f>RIGHT(Z24,2)</f>
+        <v>3)</v>
+      </c>
+    </row>
+    <row r="25" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T25" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="U25" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="V25" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T26" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="U26" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V26" s="11">
+        <v>3</v>
+      </c>
+      <c r="X26" s="19">
+        <v>3</v>
+      </c>
+      <c r="Y26" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z26" s="21" t="str">
+        <f>LEFT(Y26,5)</f>
+        <v>(1-4)</v>
+      </c>
+      <c r="AA26" s="21" t="str">
+        <f>RIGHT(Y26,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB26" s="22" t="str">
+        <f>RIGHT(Z26,2)</f>
+        <v>4)</v>
+      </c>
+    </row>
+    <row r="27" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T27" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="U27" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V27" s="11">
+        <v>4</v>
+      </c>
+      <c r="X27" s="15">
+        <v>4</v>
+      </c>
+      <c r="Y27" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z27" s="17" t="str">
+        <f>LEFT(Y27,5)</f>
+        <v>(2-4)</v>
+      </c>
+      <c r="AA27" s="17" t="str">
+        <f>RIGHT(Y27,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB27" s="18" t="str">
+        <f>RIGHT(Z27,2)</f>
+        <v>4)</v>
+      </c>
+    </row>
+    <row r="28" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T28" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="U28" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V28" s="11">
+        <v>5</v>
+      </c>
+      <c r="X28" s="19">
+        <v>5</v>
+      </c>
+      <c r="Y28" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z28" s="21" t="str">
+        <f>LEFT(Y28,5)</f>
+        <v>(3-4)</v>
+      </c>
+      <c r="AA28" s="21" t="str">
+        <f>RIGHT(Y28,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB28" s="22" t="str">
+        <f>RIGHT(Z28,2)</f>
+        <v>4)</v>
+      </c>
+    </row>
+    <row r="29" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T29" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="U29" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V29" s="10">
+        <v>8</v>
+      </c>
+      <c r="X29" s="19">
+        <v>8</v>
+      </c>
+      <c r="Y29" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z29" s="21" t="str">
+        <f>LEFT(Y29,5)</f>
+        <v>(6-4)</v>
+      </c>
+      <c r="AA29" s="21" t="str">
+        <f>RIGHT(Y29,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB29" s="22" t="str">
+        <f>RIGHT(Z29,2)</f>
+        <v>4)</v>
+      </c>
+    </row>
+    <row r="30" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T30" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="U30" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="X10">
-        <v>1</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>111</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA10" t="s">
+      <c r="V30" s="10">
+        <v>4</v>
+      </c>
+      <c r="X30" s="15">
+        <v>4</v>
+      </c>
+      <c r="Y30" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z30" s="17" t="str">
+        <f>LEFT(Y30,5)</f>
+        <v>(6-4)</v>
+      </c>
+      <c r="AA30" s="17" t="str">
+        <f>RIGHT(Y30,5)</f>
+        <v>(7-1)</v>
+      </c>
+      <c r="AB30" s="18" t="str">
+        <f>RIGHT(Z30,2)</f>
+        <v>4)</v>
+      </c>
+    </row>
+    <row r="31" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T31" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="U31" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="V31" s="10">
+        <v>9</v>
+      </c>
+      <c r="X31" s="19">
+        <v>9</v>
+      </c>
+      <c r="Y31" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z31" s="21" t="str">
+        <f>LEFT(Y31,5)</f>
+        <v>(7-4)</v>
+      </c>
+      <c r="AA31" s="21" t="str">
+        <f>RIGHT(Y31,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB31" s="22" t="str">
+        <f>RIGHT(Z31,2)</f>
+        <v>4)</v>
+      </c>
+    </row>
+    <row r="32" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T32" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="U32" s="11" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="X11">
+      <c r="V32" s="11">
+        <v>3</v>
+      </c>
+      <c r="X32" s="15">
+        <v>3</v>
+      </c>
+      <c r="Y32" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z32" s="17" t="str">
+        <f>LEFT(Y32,5)</f>
+        <v>(7-4)</v>
+      </c>
+      <c r="AA32" s="17" t="str">
+        <f>RIGHT(Y32,5)</f>
+        <v>(7-1)</v>
+      </c>
+      <c r="AB32" s="18" t="str">
+        <f>RIGHT(Z32,2)</f>
+        <v>4)</v>
+      </c>
+    </row>
+    <row r="33" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T33" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="U33" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V33" s="11">
+        <v>2</v>
+      </c>
+      <c r="X33" s="19">
+        <v>2</v>
+      </c>
+      <c r="Y33" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z33" s="21" t="str">
+        <f>LEFT(Y33,5)</f>
+        <v>(1-5)</v>
+      </c>
+      <c r="AA33" s="21" t="str">
+        <f>RIGHT(Y33,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB33" s="22" t="str">
+        <f>RIGHT(Z33,2)</f>
+        <v>5)</v>
+      </c>
+    </row>
+    <row r="34" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T34" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="U34" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V34" s="11">
+        <v>4</v>
+      </c>
+      <c r="X34" s="15">
+        <v>4</v>
+      </c>
+      <c r="Y34" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z34" s="17" t="str">
+        <f>LEFT(Y34,5)</f>
+        <v>(3-5)</v>
+      </c>
+      <c r="AA34" s="17" t="str">
+        <f>RIGHT(Y34,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB34" s="18" t="str">
+        <f>RIGHT(Z34,2)</f>
+        <v>5)</v>
+      </c>
+    </row>
+    <row r="35" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T35" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="U35" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V35" s="11">
+        <v>6</v>
+      </c>
+      <c r="X35" s="19">
+        <v>6</v>
+      </c>
+      <c r="Y35" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z35" s="21" t="str">
+        <f>LEFT(Y35,5)</f>
+        <v>(5-5)</v>
+      </c>
+      <c r="AA35" s="21" t="str">
+        <f>RIGHT(Y35,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB35" s="22" t="str">
+        <f>RIGHT(Z35,2)</f>
+        <v>5)</v>
+      </c>
+    </row>
+    <row r="36" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T36" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="U36" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V36" s="11">
         <v>7</v>
       </c>
-      <c r="Y11" t="s">
-        <v>141</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="X12">
+      <c r="X36" s="19">
+        <v>7</v>
+      </c>
+      <c r="Y36" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z36" s="21" t="str">
+        <f>LEFT(Y36,5)</f>
+        <v>(6-5)</v>
+      </c>
+      <c r="AA36" s="21" t="str">
+        <f>RIGHT(Y36,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB36" s="22" t="str">
+        <f>RIGHT(Z36,2)</f>
+        <v>5)</v>
+      </c>
+    </row>
+    <row r="37" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T37" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="U37" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="V37" s="11">
+        <v>5</v>
+      </c>
+      <c r="X37" s="15">
+        <v>5</v>
+      </c>
+      <c r="Y37" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z37" s="17" t="str">
+        <f>LEFT(Y37,5)</f>
+        <v>(6-5)</v>
+      </c>
+      <c r="AA37" s="17" t="str">
+        <f>RIGHT(Y37,5)</f>
+        <v>(7-1)</v>
+      </c>
+      <c r="AB37" s="18" t="str">
+        <f>RIGHT(Z37,2)</f>
+        <v>5)</v>
+      </c>
+    </row>
+    <row r="38" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T38" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="U38" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V38" s="11">
+        <v>1</v>
+      </c>
+      <c r="X38" s="19">
+        <v>1</v>
+      </c>
+      <c r="Y38" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z38" s="21" t="str">
+        <f>LEFT(Y38,5)</f>
+        <v>(1-6)</v>
+      </c>
+      <c r="AA38" s="21" t="str">
+        <f>RIGHT(Y38,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB38" s="22" t="str">
+        <f>RIGHT(Z38,2)</f>
+        <v>6)</v>
+      </c>
+    </row>
+    <row r="39" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T39" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="U39" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V39" s="11">
+        <v>3</v>
+      </c>
+      <c r="X39" s="15">
+        <v>3</v>
+      </c>
+      <c r="Y39" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z39" s="17" t="str">
+        <f>LEFT(Y39,5)</f>
+        <v>(3-6)</v>
+      </c>
+      <c r="AA39" s="17" t="str">
+        <f>RIGHT(Y39,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB39" s="18" t="str">
+        <f>RIGHT(Z39,2)</f>
+        <v>6)</v>
+      </c>
+    </row>
+    <row r="40" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T40" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="U40" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V40" s="11">
         <v>4</v>
       </c>
-      <c r="Y12" t="s">
-        <v>142</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="X13">
+      <c r="X40" s="19">
+        <v>4</v>
+      </c>
+      <c r="Y40" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z40" s="21" t="str">
+        <f>LEFT(Y40,5)</f>
+        <v>(4-6)</v>
+      </c>
+      <c r="AA40" s="21" t="str">
+        <f>RIGHT(Y40,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB40" s="22" t="str">
+        <f>RIGHT(Z40,2)</f>
+        <v>6)</v>
+      </c>
+    </row>
+    <row r="41" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T41" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="U41" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V41" s="11">
         <v>5</v>
       </c>
-      <c r="Y13" t="s">
-        <v>153</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="T14" t="s">
-        <v>89</v>
-      </c>
-      <c r="U14" t="s">
-        <v>86</v>
-      </c>
-      <c r="V14">
+      <c r="X41" s="19">
         <v>5</v>
       </c>
-      <c r="X14">
-        <v>5</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>89</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="T15" t="s">
-        <v>64</v>
-      </c>
-      <c r="U15" t="s">
-        <v>86</v>
-      </c>
-      <c r="V15">
+      <c r="Y41" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z41" s="21" t="str">
+        <f>LEFT(Y41,5)</f>
+        <v>(5-6)</v>
+      </c>
+      <c r="AA41" s="21" t="str">
+        <f>RIGHT(Y41,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB41" s="22" t="str">
+        <f>RIGHT(Z41,2)</f>
+        <v>6)</v>
+      </c>
+    </row>
+    <row r="42" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T42" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="U42" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V42" s="11">
         <v>6</v>
       </c>
-      <c r="X15">
+      <c r="X42" s="15">
         <v>6</v>
       </c>
-      <c r="Y15" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="T16" t="s">
-        <v>90</v>
-      </c>
-      <c r="U16" t="s">
-        <v>86</v>
-      </c>
-      <c r="V16">
+      <c r="Y42" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z42" s="17" t="str">
+        <f>LEFT(Y42,5)</f>
+        <v>(6-6)</v>
+      </c>
+      <c r="AA42" s="17" t="str">
+        <f>RIGHT(Y42,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB42" s="18" t="str">
+        <f>RIGHT(Z42,2)</f>
+        <v>6)</v>
+      </c>
+    </row>
+    <row r="43" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T43" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="U43" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V43" s="11">
+        <v>7</v>
+      </c>
+      <c r="X43" s="19">
+        <v>7</v>
+      </c>
+      <c r="Y43" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z43" s="21" t="str">
+        <f>LEFT(Y43,5)</f>
+        <v>(7-6)</v>
+      </c>
+      <c r="AA43" s="21" t="str">
+        <f>RIGHT(Y43,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB43" s="22" t="str">
+        <f>RIGHT(Z43,2)</f>
+        <v>6)</v>
+      </c>
+    </row>
+    <row r="44" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T44" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="U44" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V44" s="11">
+        <v>1</v>
+      </c>
+      <c r="X44" s="15">
+        <v>1</v>
+      </c>
+      <c r="Y44" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z44" s="17" t="str">
+        <f>LEFT(Y44,5)</f>
+        <v>(2-7)</v>
+      </c>
+      <c r="AA44" s="17" t="str">
+        <f>RIGHT(Y44,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB44" s="18" t="str">
+        <f>RIGHT(Z44,2)</f>
+        <v>7)</v>
+      </c>
+    </row>
+    <row r="45" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T45" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="U45" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V45" s="11">
+        <v>2</v>
+      </c>
+      <c r="X45" s="19">
+        <v>2</v>
+      </c>
+      <c r="Y45" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z45" s="21" t="str">
+        <f>LEFT(Y45,5)</f>
+        <v>(3-7)</v>
+      </c>
+      <c r="AA45" s="21" t="str">
+        <f>RIGHT(Y45,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB45" s="22" t="str">
+        <f>RIGHT(Z45,2)</f>
+        <v>7)</v>
+      </c>
+    </row>
+    <row r="46" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T46" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="U46" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V46" s="11">
+        <v>3</v>
+      </c>
+      <c r="X46" s="15">
+        <v>3</v>
+      </c>
+      <c r="Y46" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z46" s="17" t="str">
+        <f>LEFT(Y46,5)</f>
+        <v>(4-7)</v>
+      </c>
+      <c r="AA46" s="17" t="str">
+        <f>RIGHT(Y46,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB46" s="18" t="str">
+        <f>RIGHT(Z46,2)</f>
+        <v>7)</v>
+      </c>
+    </row>
+    <row r="47" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T47" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="U47" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V47" s="11">
+        <v>4</v>
+      </c>
+      <c r="X47" s="19">
+        <v>4</v>
+      </c>
+      <c r="Y47" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z47" s="21" t="str">
+        <f>LEFT(Y47,5)</f>
+        <v>(5-7)</v>
+      </c>
+      <c r="AA47" s="21" t="str">
+        <f>RIGHT(Y47,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB47" s="22" t="str">
+        <f>RIGHT(Z47,2)</f>
+        <v>7)</v>
+      </c>
+    </row>
+    <row r="48" spans="20:28" x14ac:dyDescent="0.3">
+      <c r="T48" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="U48" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="V48" s="11">
         <v>8</v>
       </c>
-      <c r="X16">
+      <c r="X48" s="6">
         <v>8</v>
       </c>
-      <c r="Y16" t="s">
-        <v>114</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T17" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="U17" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="V17" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T18" t="s">
-        <v>91</v>
-      </c>
-      <c r="U18" t="s">
-        <v>87</v>
-      </c>
-      <c r="V18">
-        <v>1</v>
-      </c>
-      <c r="X18">
-        <v>1</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>91</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T19" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="U19" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="V19" s="5">
-        <v>11</v>
-      </c>
-      <c r="X19">
-        <v>4</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T20" t="s">
-        <v>92</v>
-      </c>
-      <c r="U20" t="s">
-        <v>86</v>
-      </c>
-      <c r="V20">
-        <v>4</v>
-      </c>
-      <c r="X20">
-        <v>4</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>116</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T21" t="s">
-        <v>93</v>
-      </c>
-      <c r="U21" t="s">
-        <v>86</v>
-      </c>
-      <c r="V21">
-        <v>6</v>
-      </c>
-      <c r="X21">
-        <v>6</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T22" t="s">
-        <v>69</v>
-      </c>
-      <c r="U22" t="s">
-        <v>86</v>
-      </c>
-      <c r="V22">
-        <v>7</v>
-      </c>
-      <c r="X22">
-        <v>7</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>118</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T23" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="U23" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="V23" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T24" t="s">
-        <v>70</v>
-      </c>
-      <c r="U24" t="s">
-        <v>86</v>
-      </c>
-      <c r="V24">
-        <v>8</v>
-      </c>
-      <c r="X24">
-        <v>8</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T25" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="U25" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="V25" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T26" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="U26" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="V26" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T27" t="s">
-        <v>94</v>
-      </c>
-      <c r="U27" t="s">
-        <v>86</v>
-      </c>
-      <c r="V27">
-        <v>9</v>
-      </c>
-      <c r="X27">
-        <v>9</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T28" t="s">
-        <v>95</v>
-      </c>
-      <c r="U28" t="s">
-        <v>87</v>
-      </c>
-      <c r="V28">
-        <v>2</v>
-      </c>
-      <c r="X28">
-        <v>2</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>121</v>
-      </c>
-      <c r="Z28" t="s">
-        <v>95</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T29" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="U29" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="V29" s="5">
-        <v>10</v>
-      </c>
-      <c r="X29">
-        <v>4</v>
-      </c>
-      <c r="Y29" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="Z29" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="X30">
-        <v>3</v>
-      </c>
-      <c r="Y30" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="Z30" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="X31">
-        <v>5</v>
-      </c>
-      <c r="Y31" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA31" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T32" t="s">
-        <v>71</v>
-      </c>
-      <c r="U32" t="s">
-        <v>86</v>
-      </c>
-      <c r="V32">
-        <v>3</v>
-      </c>
-      <c r="X32">
-        <v>3</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>122</v>
-      </c>
-      <c r="Z32" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA32" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T33" t="s">
-        <v>72</v>
-      </c>
-      <c r="U33" t="s">
-        <v>86</v>
-      </c>
-      <c r="V33">
-        <v>4</v>
-      </c>
-      <c r="X33">
-        <v>4</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>123</v>
-      </c>
-      <c r="Z33" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T34" t="s">
-        <v>73</v>
-      </c>
-      <c r="U34" t="s">
-        <v>86</v>
-      </c>
-      <c r="V34">
-        <v>5</v>
-      </c>
-      <c r="X34">
-        <v>5</v>
-      </c>
-      <c r="Y34" t="s">
-        <v>124</v>
-      </c>
-      <c r="Z34" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA34" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T35" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="U35" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="V35" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T36" t="s">
-        <v>76</v>
-      </c>
-      <c r="U36" t="s">
-        <v>86</v>
-      </c>
-      <c r="V36" s="5">
-        <v>8</v>
-      </c>
-      <c r="X36">
-        <v>10</v>
-      </c>
-      <c r="Y36" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z36" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA36" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T37" t="s">
-        <v>96</v>
-      </c>
-      <c r="U37" t="s">
-        <v>87</v>
-      </c>
-      <c r="V37">
-        <v>3</v>
-      </c>
-      <c r="X37">
-        <v>3</v>
-      </c>
-      <c r="Y37" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z37" t="s">
-        <v>96</v>
-      </c>
-      <c r="AA37" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T38" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="U38" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="V38" s="5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T39" t="s">
-        <v>97</v>
-      </c>
-      <c r="U39" t="s">
-        <v>86</v>
-      </c>
-      <c r="V39">
-        <v>2</v>
-      </c>
-      <c r="X39">
-        <v>4</v>
-      </c>
-      <c r="Y39" t="s">
-        <v>147</v>
-      </c>
-      <c r="Z39" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA39" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="40" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T40" t="s">
-        <v>98</v>
-      </c>
-      <c r="U40" t="s">
-        <v>86</v>
-      </c>
-      <c r="V40">
-        <v>4</v>
-      </c>
-      <c r="X40">
-        <v>4</v>
-      </c>
-      <c r="Y40" t="s">
-        <v>155</v>
-      </c>
-      <c r="Z40" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA40" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T41" t="s">
-        <v>79</v>
-      </c>
-      <c r="U41" t="s">
-        <v>86</v>
-      </c>
-      <c r="V41">
-        <v>6</v>
-      </c>
-      <c r="X41">
-        <v>2</v>
-      </c>
-      <c r="Y41" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z41" t="s">
-        <v>97</v>
-      </c>
-      <c r="AA41" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="42" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T42" t="s">
-        <v>80</v>
-      </c>
-      <c r="U42" t="s">
-        <v>87</v>
-      </c>
-      <c r="V42">
-        <v>5</v>
-      </c>
-      <c r="X42">
-        <v>4</v>
-      </c>
-      <c r="Y42" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z42" t="s">
-        <v>98</v>
-      </c>
-      <c r="AA42" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T43" t="s">
-        <v>80</v>
-      </c>
-      <c r="U43" t="s">
-        <v>86</v>
-      </c>
-      <c r="V43">
-        <v>7</v>
-      </c>
-      <c r="X43">
-        <v>12</v>
-      </c>
-      <c r="Y43" t="s">
-        <v>129</v>
-      </c>
-      <c r="Z43" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T44" t="s">
-        <v>59</v>
-      </c>
-      <c r="U44" t="s">
-        <v>86</v>
-      </c>
-      <c r="V44">
-        <v>1</v>
-      </c>
-      <c r="X44">
-        <v>11</v>
-      </c>
-      <c r="Y44" t="s">
-        <v>130</v>
-      </c>
-      <c r="Z44" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA44" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T45" t="s">
-        <v>82</v>
-      </c>
-      <c r="U45" t="s">
-        <v>86</v>
-      </c>
-      <c r="V45">
-        <v>3</v>
-      </c>
-      <c r="X45">
-        <v>6</v>
-      </c>
-      <c r="Y45" t="s">
-        <v>148</v>
-      </c>
-      <c r="Z45" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA45" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T46" t="s">
-        <v>83</v>
-      </c>
-      <c r="U46" t="s">
-        <v>86</v>
-      </c>
-      <c r="V46">
-        <v>4</v>
-      </c>
-      <c r="X46">
-        <v>5</v>
-      </c>
-      <c r="Y46" t="s">
-        <v>149</v>
-      </c>
-      <c r="Z46" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA46" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T47" t="s">
-        <v>105</v>
-      </c>
-      <c r="U47" t="s">
-        <v>86</v>
-      </c>
-      <c r="V47">
-        <v>5</v>
-      </c>
-      <c r="X47">
-        <v>6</v>
-      </c>
-      <c r="Y47" t="s">
-        <v>156</v>
-      </c>
-      <c r="Z47" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA47" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="48" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T48" t="s">
-        <v>84</v>
-      </c>
-      <c r="U48" t="s">
-        <v>86</v>
-      </c>
-      <c r="V48">
-        <v>6</v>
-      </c>
-      <c r="X48">
-        <v>5</v>
-      </c>
-      <c r="Y48" t="s">
-        <v>157</v>
-      </c>
-      <c r="Z48" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA48" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T49" t="s">
-        <v>99</v>
-      </c>
-      <c r="U49" t="s">
-        <v>86</v>
-      </c>
-      <c r="V49">
-        <v>7</v>
-      </c>
-      <c r="X49">
-        <v>1</v>
-      </c>
-      <c r="Y49" t="s">
-        <v>131</v>
-      </c>
-      <c r="Z49" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA49" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="50" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T50" t="s">
-        <v>100</v>
-      </c>
-      <c r="U50" t="s">
-        <v>86</v>
-      </c>
-      <c r="V50">
-        <v>1</v>
-      </c>
-      <c r="X50">
-        <v>3</v>
-      </c>
-      <c r="Y50" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z50" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA50" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T51" t="s">
-        <v>101</v>
-      </c>
-      <c r="U51" t="s">
-        <v>86</v>
-      </c>
-      <c r="V51">
-        <v>2</v>
-      </c>
-      <c r="X51">
-        <v>4</v>
-      </c>
-      <c r="Y51" t="s">
-        <v>133</v>
-      </c>
-      <c r="Z51" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA51" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="52" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T52" t="s">
-        <v>102</v>
-      </c>
-      <c r="U52" t="s">
-        <v>86</v>
-      </c>
-      <c r="V52">
-        <v>3</v>
-      </c>
-      <c r="X52">
-        <v>12</v>
-      </c>
-      <c r="Y52" t="s">
-        <v>134</v>
-      </c>
-      <c r="Z52" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA52" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="53" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T53" t="s">
-        <v>103</v>
-      </c>
-      <c r="U53" t="s">
-        <v>86</v>
-      </c>
-      <c r="V53">
-        <v>4</v>
-      </c>
-      <c r="X53">
-        <v>13</v>
-      </c>
-      <c r="Y53" t="s">
-        <v>135</v>
-      </c>
-      <c r="Z53" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA53" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="T54" t="s">
-        <v>104</v>
-      </c>
-      <c r="U54" t="s">
-        <v>86</v>
-      </c>
-      <c r="V54">
-        <v>8</v>
-      </c>
-      <c r="X54">
-        <v>6</v>
-      </c>
-      <c r="Y54" t="s">
-        <v>150</v>
-      </c>
-      <c r="Z54" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA54" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="55" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="X55">
-        <v>7</v>
-      </c>
-      <c r="Y55" t="s">
-        <v>151</v>
-      </c>
-      <c r="Z55" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA55" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="56" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="X56">
-        <v>4</v>
-      </c>
-      <c r="Y56" t="s">
-        <v>158</v>
-      </c>
-      <c r="Z56" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA56" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="57" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="X57">
-        <v>6</v>
-      </c>
-      <c r="Y57" t="s">
-        <v>159</v>
-      </c>
-      <c r="Z57" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA57" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="58" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="X58">
-        <v>7</v>
-      </c>
-      <c r="Y58" t="s">
-        <v>160</v>
-      </c>
-      <c r="Z58" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA58" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="59" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="X59">
-        <v>1</v>
-      </c>
-      <c r="Y59" t="s">
-        <v>136</v>
-      </c>
-      <c r="Z59" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA59" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="60" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="X60">
-        <v>2</v>
-      </c>
-      <c r="Y60" t="s">
-        <v>137</v>
-      </c>
-      <c r="Z60" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA60" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="61" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="X61">
-        <v>3</v>
-      </c>
-      <c r="Y61" t="s">
-        <v>138</v>
-      </c>
-      <c r="Z61" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA61" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="62" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="X62">
-        <v>4</v>
-      </c>
-      <c r="Y62" t="s">
-        <v>139</v>
-      </c>
-      <c r="Z62" t="s">
-        <v>103</v>
-      </c>
-      <c r="AA62" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="63" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="X63">
-        <v>14</v>
-      </c>
-      <c r="Y63" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z63" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA63" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="64" spans="20:27" x14ac:dyDescent="0.3">
-      <c r="X64">
-        <v>8</v>
-      </c>
-      <c r="Y64" t="s">
-        <v>152</v>
-      </c>
-      <c r="Z64" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA64" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="65" spans="24:27" x14ac:dyDescent="0.3">
-      <c r="X65">
-        <v>8</v>
-      </c>
-      <c r="Y65" t="s">
-        <v>161</v>
-      </c>
-      <c r="Z65" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA65" t="s">
-        <v>87</v>
+      <c r="Y48" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z48" s="8" t="str">
+        <f>LEFT(Y48,5)</f>
+        <v>(7-7)</v>
+      </c>
+      <c r="AA48" s="8" t="str">
+        <f>RIGHT(Y48,5)</f>
+        <v>(1-7)</v>
+      </c>
+      <c r="AB48" s="9" t="str">
+        <f>RIGHT(Z48,2)</f>
+        <v>7)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>